<commit_message>
testing adjust portion api
</commit_message>
<xml_diff>
--- a/backend/data/Meal Builder BF.xlsx
+++ b/backend/data/Meal Builder BF.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjaysaroop/Desktop/Digital/Cuore&gt;/Content/Cuore Nutrition/Breakfast &amp; Snacks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO-PF0XZXLK\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00898BF1-6EDC-D449-A643-DDD24A0305D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="500" windowWidth="22080" windowHeight="16120" activeTab="1" xr2:uid="{17354DCE-A742-B34C-8AE4-DA88639DB2B5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6430"/>
   </bookViews>
   <sheets>
     <sheet name="Indian" sheetId="4" r:id="rId1"/>
     <sheet name="Global" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="179">
   <si>
     <t>Recommended Calories for Breakfast</t>
   </si>
@@ -549,16 +548,40 @@
   </si>
   <si>
     <t>1 Khubz</t>
+  </si>
+  <si>
+    <t>(N12/$N$17)*$D$3/M12*L12</t>
+  </si>
+  <si>
+    <t>(N13/$N$17)*$D$3/M13*L13</t>
+  </si>
+  <si>
+    <t>(N14/$N$17)*$D$3/M14*L14</t>
+  </si>
+  <si>
+    <t>(N15/$N$17)*$D$3/M15*L15</t>
+  </si>
+  <si>
+    <t>MROUND(O12,0.25)</t>
+  </si>
+  <si>
+    <t>MROUND(O13,0.25)</t>
+  </si>
+  <si>
+    <t>MROUND(O14,0.25)</t>
+  </si>
+  <si>
+    <t>MROUND(O15,0.25)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -800,7 +823,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -951,6 +974,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -969,7 +993,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1341,27 +1365,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD5DD28-AFFC-FD49-9975-DD17AC460F10}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J91"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="31.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="1"/>
+    <col min="2" max="2" width="31.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.84375" style="2"/>
+    <col min="5" max="5" width="7.15234375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="20.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="5.69140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.84375" style="1"/>
+    <col min="9" max="9" width="20.4609375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1370,7 +1394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1382,47 +1406,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
       <c r="G4" s="3"/>
       <c r="H4" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9">
       <c r="B6" s="8"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="59" t="s">
+    <row r="7" spans="2:9">
+      <c r="B7" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61"/>
-    </row>
-    <row r="8" spans="2:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+    </row>
+    <row r="8" spans="2:9" ht="29">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1436,13 +1460,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9">
       <c r="B9" s="12" t="s">
         <v>150</v>
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9">
       <c r="B10" s="13" t="s">
         <v>91</v>
       </c>
@@ -1466,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9">
       <c r="B11" s="13" t="s">
         <v>92</v>
       </c>
@@ -1490,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9">
       <c r="B12" s="13" t="s">
         <v>93</v>
       </c>
@@ -1514,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9">
       <c r="B13" s="13" t="s">
         <v>94</v>
       </c>
@@ -1538,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9">
       <c r="B14" s="13" t="s">
         <v>95</v>
       </c>
@@ -1562,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9">
       <c r="B15" s="13"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1571,7 +1595,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="56"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9">
       <c r="B16" s="12" t="s">
         <v>151</v>
       </c>
@@ -1581,7 +1605,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="56"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9">
       <c r="B17" s="13" t="s">
         <v>98</v>
       </c>
@@ -1603,7 +1627,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9">
       <c r="B18" s="13" t="s">
         <v>99</v>
       </c>
@@ -1625,7 +1649,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9">
       <c r="B19" s="13" t="s">
         <v>100</v>
       </c>
@@ -1647,7 +1671,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9">
       <c r="B20" s="13" t="s">
         <v>101</v>
       </c>
@@ -1669,7 +1693,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9">
       <c r="B21" s="13" t="s">
         <v>102</v>
       </c>
@@ -1691,7 +1715,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9">
       <c r="B22" s="13" t="s">
         <v>103</v>
       </c>
@@ -1713,7 +1737,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9">
       <c r="B23" s="13" t="s">
         <v>104</v>
       </c>
@@ -1735,7 +1759,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9">
       <c r="B24" s="13" t="s">
         <v>105</v>
       </c>
@@ -1757,7 +1781,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9">
       <c r="B25" s="13" t="s">
         <v>106</v>
       </c>
@@ -1779,7 +1803,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9">
       <c r="B26" s="13" t="s">
         <v>107</v>
       </c>
@@ -1801,7 +1825,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9">
       <c r="B27" s="13" t="s">
         <v>137</v>
       </c>
@@ -1823,16 +1847,16 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" customFormat="1" ht="15.5">
       <c r="H28" s="57"/>
     </row>
-    <row r="29" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" customFormat="1" ht="15.5">
       <c r="B29" s="12" t="s">
         <v>152</v>
       </c>
       <c r="H29" s="57"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9">
       <c r="B30" s="13" t="s">
         <v>108</v>
       </c>
@@ -1856,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9">
       <c r="B31" s="13" t="s">
         <v>109</v>
       </c>
@@ -1880,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9">
       <c r="B32" s="13" t="s">
         <v>110</v>
       </c>
@@ -1904,7 +1928,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9">
       <c r="B33" s="13" t="s">
         <v>112</v>
       </c>
@@ -1926,7 +1950,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9">
       <c r="B34" s="13" t="s">
         <v>113</v>
       </c>
@@ -1948,7 +1972,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9">
       <c r="B35" s="13" t="s">
         <v>114</v>
       </c>
@@ -1970,7 +1994,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9">
       <c r="B36" s="13" t="s">
         <v>115</v>
       </c>
@@ -1992,17 +2016,17 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="37" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" customFormat="1" ht="15.5">
       <c r="H37" s="57"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9">
       <c r="B38" s="12" t="s">
         <v>153</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="56"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9">
       <c r="B39" s="13" t="s">
         <v>131</v>
       </c>
@@ -2024,7 +2048,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9">
       <c r="B40" s="13" t="s">
         <v>132</v>
       </c>
@@ -2046,7 +2070,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9">
       <c r="B41" s="13" t="s">
         <v>133</v>
       </c>
@@ -2068,7 +2092,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9">
       <c r="B42" s="13" t="s">
         <v>134</v>
       </c>
@@ -2090,7 +2114,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9">
       <c r="B43" s="13" t="s">
         <v>135</v>
       </c>
@@ -2112,7 +2136,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9">
       <c r="B44" s="13" t="s">
         <v>136</v>
       </c>
@@ -2134,7 +2158,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9">
       <c r="B45" s="13" t="s">
         <v>138</v>
       </c>
@@ -2156,7 +2180,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9">
       <c r="B46" s="13" t="s">
         <v>139</v>
       </c>
@@ -2178,16 +2202,16 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="47" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9" customFormat="1" ht="15.5">
       <c r="H47" s="57"/>
     </row>
-    <row r="48" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9" customFormat="1" ht="15.5">
       <c r="B48" s="12" t="s">
         <v>154</v>
       </c>
       <c r="H48" s="57"/>
     </row>
-    <row r="49" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" customFormat="1" ht="15.5">
       <c r="B49" s="13" t="s">
         <v>125</v>
       </c>
@@ -2211,7 +2235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" customFormat="1" ht="15.5">
       <c r="B50" s="13" t="s">
         <v>126</v>
       </c>
@@ -2235,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" customFormat="1" ht="15.5">
       <c r="B51" s="13" t="s">
         <v>127</v>
       </c>
@@ -2259,7 +2283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" customFormat="1" ht="15.5">
       <c r="B52" s="13" t="s">
         <v>149</v>
       </c>
@@ -2277,16 +2301,16 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="53" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" customFormat="1" ht="15.5">
       <c r="H53" s="57"/>
     </row>
-    <row r="54" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" customFormat="1" ht="15.5">
       <c r="B54" s="12" t="s">
         <v>155</v>
       </c>
       <c r="H54" s="57"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9">
       <c r="B55" s="13" t="s">
         <v>116</v>
       </c>
@@ -2310,7 +2334,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9">
       <c r="B56" s="13" t="s">
         <v>117</v>
       </c>
@@ -2334,7 +2358,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:9">
       <c r="B57" s="13" t="s">
         <v>118</v>
       </c>
@@ -2358,7 +2382,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9">
       <c r="B58" s="13" t="s">
         <v>119</v>
       </c>
@@ -2382,7 +2406,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9">
       <c r="B59" s="13" t="s">
         <v>146</v>
       </c>
@@ -2400,7 +2424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:9">
       <c r="B60" s="13" t="s">
         <v>128</v>
       </c>
@@ -2424,7 +2448,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:9">
       <c r="B61" s="13" t="s">
         <v>129</v>
       </c>
@@ -2448,7 +2472,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="62" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:9" customFormat="1" ht="15.5">
       <c r="B62" s="13" t="s">
         <v>130</v>
       </c>
@@ -2472,10 +2496,10 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="63" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:9" customFormat="1" ht="15.5">
       <c r="H63" s="57"/>
     </row>
-    <row r="64" spans="2:9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:9" customFormat="1" ht="15.5">
       <c r="B64" s="12" t="s">
         <v>156</v>
       </c>
@@ -2487,7 +2511,7 @@
       <c r="H64" s="56"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:10" customFormat="1" ht="15.5">
       <c r="B65" s="13" t="s">
         <v>124</v>
       </c>
@@ -2511,7 +2535,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="66" spans="2:10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:10" customFormat="1" ht="15.5">
       <c r="B66" s="13" t="s">
         <v>141</v>
       </c>
@@ -2533,7 +2557,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="67" spans="2:10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:10" customFormat="1" ht="15.5">
       <c r="B67" s="13" t="s">
         <v>142</v>
       </c>
@@ -2555,7 +2579,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="68" spans="2:10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:10" customFormat="1" ht="15.5">
       <c r="B68" s="13" t="s">
         <v>143</v>
       </c>
@@ -2577,7 +2601,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="69" spans="2:10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:10" customFormat="1" ht="15.5">
       <c r="B69" s="13" t="s">
         <v>144</v>
       </c>
@@ -2599,7 +2623,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="70" spans="2:10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:10" customFormat="1" ht="15.5">
       <c r="B70" s="13" t="s">
         <v>122</v>
       </c>
@@ -2623,7 +2647,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:10">
       <c r="B71" s="13" t="s">
         <v>123</v>
       </c>
@@ -2647,7 +2671,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="72" spans="2:10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:10" customFormat="1" ht="15.5">
       <c r="B72" s="13" t="s">
         <v>111</v>
       </c>
@@ -2669,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:10">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -2677,7 +2701,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="56"/>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:10">
       <c r="B74" s="12" t="s">
         <v>157</v>
       </c>
@@ -2687,7 +2711,7 @@
       <c r="G74" s="3"/>
       <c r="H74" s="56"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:10">
       <c r="B75" s="13" t="s">
         <v>120</v>
       </c>
@@ -2711,7 +2735,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:10">
       <c r="B76" s="13" t="s">
         <v>140</v>
       </c>
@@ -2735,7 +2759,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:10">
       <c r="B77" s="13" t="s">
         <v>121</v>
       </c>
@@ -2759,7 +2783,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:10">
       <c r="B78" s="13"/>
       <c r="C78" s="15"/>
       <c r="D78" s="15"/>
@@ -2768,13 +2792,13 @@
       <c r="G78" s="3"/>
       <c r="H78" s="56"/>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:10">
       <c r="B79" s="49" t="s">
         <v>158</v>
       </c>
       <c r="H79" s="56"/>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:10">
       <c r="B80" s="13" t="s">
         <v>45</v>
       </c>
@@ -2801,7 +2825,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:10">
       <c r="B81" s="13" t="s">
         <v>145</v>
       </c>
@@ -2828,7 +2852,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:10">
       <c r="B82" s="13" t="s">
         <v>96</v>
       </c>
@@ -2855,7 +2879,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:10">
       <c r="B83" s="13" t="s">
         <v>44</v>
       </c>
@@ -2882,7 +2906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:10">
       <c r="B84" s="13" t="s">
         <v>47</v>
       </c>
@@ -2909,7 +2933,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:10">
       <c r="B85" s="13" t="s">
         <v>96</v>
       </c>
@@ -2936,7 +2960,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:10">
       <c r="B86" s="13" t="s">
         <v>97</v>
       </c>
@@ -2963,14 +2987,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:10">
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:10">
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -2997,35 +3021,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116E5E29-5736-8846-B95E-0169515F6161}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="31.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="19.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.84375" style="1"/>
+    <col min="2" max="2" width="31.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.15234375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.69140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.84375" style="1"/>
+    <col min="9" max="9" width="19.4609375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.84375" style="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="10.4609375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="23.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.84375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -3034,7 +3058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:19">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -3048,7 +3072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:19">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -3062,7 +3086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -3074,31 +3098,31 @@
       <c r="E5" s="9"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19">
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:19">
       <c r="B7" s="8"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="59" t="s">
+    <row r="8" spans="2:19">
+      <c r="B8" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61"/>
-    </row>
-    <row r="9" spans="2:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+    </row>
+    <row r="9" spans="2:19" ht="29">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="62"/>
+      <c r="D9" s="63"/>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
@@ -3112,13 +3136,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:19">
       <c r="B10" s="12" t="s">
         <v>159</v>
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="2:19" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:19" ht="38" customHeight="1">
       <c r="B11" s="13" t="s">
         <v>37</v>
       </c>
@@ -3163,7 +3187,7 @@
       <c r="Q11" s="22"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:19">
       <c r="B12" s="13" t="s">
         <v>38</v>
       </c>
@@ -3202,19 +3226,17 @@
         <f>I12</f>
         <v>1</v>
       </c>
-      <c r="O12" s="27">
-        <f>(N12/$N$17)*$D$3/M12*L12</f>
-        <v>0.38461538461538469</v>
-      </c>
-      <c r="P12" s="28">
-        <f>MROUND(O12,0.25)</f>
-        <v>0.5</v>
+      <c r="O12" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="P12" s="28" t="s">
+        <v>175</v>
       </c>
       <c r="Q12" s="22"/>
       <c r="R12" s="29"/>
       <c r="S12" s="30"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:19">
       <c r="B13" s="13" t="s">
         <v>39</v>
       </c>
@@ -3253,19 +3275,17 @@
         <f>I21</f>
         <v>1</v>
       </c>
-      <c r="O13" s="27">
-        <f>(N13/$N$17)*$D$3/M13*L13</f>
-        <v>0.32967032967032972</v>
-      </c>
-      <c r="P13" s="28">
-        <f t="shared" ref="P13:P15" si="0">MROUND(O13,0.25)</f>
-        <v>0.25</v>
+      <c r="O13" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="P13" s="28" t="s">
+        <v>176</v>
       </c>
       <c r="Q13" s="22"/>
       <c r="R13" s="29"/>
       <c r="S13" s="30"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:19">
       <c r="B14" s="13" t="s">
         <v>40</v>
       </c>
@@ -3304,19 +3324,17 @@
         <f>I40</f>
         <v>0.3</v>
       </c>
-      <c r="O14" s="27">
-        <f>(N14/$N$17)*$D$3/M14*L14</f>
-        <v>1.7307692307692311</v>
-      </c>
-      <c r="P14" s="28">
-        <f t="shared" si="0"/>
-        <v>1.75</v>
+      <c r="O14" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="P14" s="28" t="s">
+        <v>177</v>
       </c>
       <c r="Q14" s="22"/>
       <c r="R14" s="29"/>
       <c r="S14" s="30"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:19">
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
@@ -3338,19 +3356,17 @@
         <f>I67</f>
         <v>0.3</v>
       </c>
-      <c r="O15" s="27">
-        <f>(N15/$N$17)*$D$3/M15*L15</f>
-        <v>0.36437246963562758</v>
-      </c>
-      <c r="P15" s="28">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
+      <c r="O15" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="P15" s="28" t="s">
+        <v>178</v>
       </c>
       <c r="Q15" s="22"/>
       <c r="R15" s="29"/>
       <c r="S15" s="30"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:19">
       <c r="B16" s="12" t="s">
         <v>160</v>
       </c>
@@ -3364,7 +3380,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:18">
       <c r="B17" s="13" t="s">
         <v>49</v>
       </c>
@@ -3391,14 +3407,14 @@
       <c r="L17" s="2"/>
       <c r="M17" s="37"/>
       <c r="N17" s="38">
-        <f>SUM(N12:N16)</f>
+        <f>SUM(N12:N15)</f>
         <v>2.5999999999999996</v>
       </c>
       <c r="O17" s="20"/>
       <c r="P17" s="39"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:18">
       <c r="B18" s="13" t="s">
         <v>50</v>
       </c>
@@ -3423,7 +3439,7 @@
       </c>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:18">
       <c r="B19" s="13" t="s">
         <v>51</v>
       </c>
@@ -3451,7 +3467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:18">
       <c r="B20" s="13" t="s">
         <v>52</v>
       </c>
@@ -3476,7 +3492,7 @@
       </c>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:18">
       <c r="B21" s="13" t="s">
         <v>53</v>
       </c>
@@ -3501,7 +3517,7 @@
       </c>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:18">
       <c r="B22" s="13" t="s">
         <v>54</v>
       </c>
@@ -3526,7 +3542,7 @@
       </c>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:18">
       <c r="B23" s="13" t="s">
         <v>55</v>
       </c>
@@ -3551,21 +3567,22 @@
       </c>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:18">
       <c r="B24" s="13"/>
       <c r="C24" s="14"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="N24" s="58"/>
+    </row>
+    <row r="25" spans="2:18">
       <c r="B25" s="12" t="s">
         <v>161</v>
       </c>
       <c r="C25" s="14"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:18">
       <c r="B26" s="13" t="s">
         <v>56</v>
       </c>
@@ -3590,7 +3607,7 @@
       </c>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:18">
       <c r="B27" s="13" t="s">
         <v>57</v>
       </c>
@@ -3615,7 +3632,7 @@
       </c>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:18">
       <c r="B28" s="13" t="s">
         <v>58</v>
       </c>
@@ -3638,7 +3655,7 @@
       </c>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:18">
       <c r="B29" s="13" t="s">
         <v>59</v>
       </c>
@@ -3661,7 +3678,7 @@
       </c>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:18">
       <c r="B30" s="13" t="s">
         <v>60</v>
       </c>
@@ -3684,7 +3701,7 @@
       </c>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:18">
       <c r="B31" s="13" t="s">
         <v>61</v>
       </c>
@@ -3707,7 +3724,7 @@
       </c>
       <c r="J31" s="17"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:18">
       <c r="B32" s="13" t="s">
         <v>62</v>
       </c>
@@ -3730,7 +3747,7 @@
       </c>
       <c r="J32" s="17"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10">
       <c r="B33" s="13" t="s">
         <v>63</v>
       </c>
@@ -3755,7 +3772,7 @@
       </c>
       <c r="J33" s="17"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10">
       <c r="B34" s="13" t="s">
         <v>64</v>
       </c>
@@ -3780,7 +3797,7 @@
       </c>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10">
       <c r="B35" s="13" t="s">
         <v>168</v>
       </c>
@@ -3805,7 +3822,7 @@
       </c>
       <c r="J35" s="17"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10">
       <c r="B36" s="13" t="s">
         <v>169</v>
       </c>
@@ -3828,7 +3845,7 @@
       </c>
       <c r="J36" s="17"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10">
       <c r="B37" s="13" t="s">
         <v>170</v>
       </c>
@@ -3851,21 +3868,21 @@
       </c>
       <c r="J37" s="17"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10">
       <c r="B38" s="44"/>
       <c r="C38" s="14"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10">
       <c r="B39" s="12" t="s">
         <v>165</v>
       </c>
       <c r="C39" s="14"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10">
       <c r="B40" s="13" t="s">
         <v>65</v>
       </c>
@@ -3888,7 +3905,7 @@
       </c>
       <c r="J40" s="17"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10">
       <c r="B41" s="13" t="s">
         <v>66</v>
       </c>
@@ -3911,7 +3928,7 @@
       </c>
       <c r="J41" s="17"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10">
       <c r="B42" s="13" t="s">
         <v>67</v>
       </c>
@@ -3932,7 +3949,7 @@
       </c>
       <c r="J42" s="17"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10">
       <c r="B43" s="13" t="s">
         <v>68</v>
       </c>
@@ -3955,7 +3972,7 @@
       </c>
       <c r="J43" s="17"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10">
       <c r="B44" s="13" t="s">
         <v>69</v>
       </c>
@@ -3978,7 +3995,7 @@
       </c>
       <c r="J44" s="17"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10">
       <c r="B45" s="13" t="s">
         <v>147</v>
       </c>
@@ -4003,7 +4020,7 @@
       </c>
       <c r="J45" s="17"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10">
       <c r="B46" s="13" t="s">
         <v>70</v>
       </c>
@@ -4026,7 +4043,7 @@
       </c>
       <c r="J46" s="17"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10">
       <c r="B47" s="13" t="s">
         <v>148</v>
       </c>
@@ -4051,7 +4068,7 @@
       </c>
       <c r="J47" s="17"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10">
       <c r="B48" s="13" t="s">
         <v>71</v>
       </c>
@@ -4074,7 +4091,7 @@
       </c>
       <c r="J48" s="17"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10">
       <c r="B49" s="13" t="s">
         <v>72</v>
       </c>
@@ -4097,7 +4114,7 @@
       </c>
       <c r="J49" s="17"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10">
       <c r="B50" s="13" t="s">
         <v>73</v>
       </c>
@@ -4120,7 +4137,7 @@
       </c>
       <c r="J50" s="17"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10">
       <c r="B51" s="13" t="s">
         <v>166</v>
       </c>
@@ -4143,7 +4160,7 @@
       </c>
       <c r="J51" s="17"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10">
       <c r="B52" s="13" t="s">
         <v>167</v>
       </c>
@@ -4166,7 +4183,7 @@
       </c>
       <c r="J52" s="17"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:10">
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
       <c r="D53" s="15"/>
@@ -4174,7 +4191,7 @@
       <c r="F53" s="48"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10">
       <c r="B54" s="49" t="s">
         <v>162</v>
       </c>
@@ -4182,7 +4199,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="50"/>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:10">
       <c r="B55" s="13" t="s">
         <v>74</v>
       </c>
@@ -4207,7 +4224,7 @@
       </c>
       <c r="J55" s="17"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:10">
       <c r="B56" s="13" t="s">
         <v>75</v>
       </c>
@@ -4232,7 +4249,7 @@
       </c>
       <c r="J56" s="17"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10">
       <c r="B57" s="13" t="s">
         <v>76</v>
       </c>
@@ -4257,7 +4274,7 @@
       </c>
       <c r="J57" s="17"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:10">
       <c r="B58" s="13" t="s">
         <v>77</v>
       </c>
@@ -4282,7 +4299,7 @@
       </c>
       <c r="J58" s="17"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:10">
       <c r="B59" s="13" t="s">
         <v>78</v>
       </c>
@@ -4307,7 +4324,7 @@
       </c>
       <c r="J59" s="17"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10">
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
       <c r="D60" s="15"/>
@@ -4315,7 +4332,7 @@
       <c r="F60" s="32"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10">
       <c r="B61" s="49" t="s">
         <v>163</v>
       </c>
@@ -4325,7 +4342,7 @@
       <c r="F61" s="32"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:10">
       <c r="B62" s="13" t="s">
         <v>79</v>
       </c>
@@ -4350,7 +4367,7 @@
       </c>
       <c r="J62" s="17"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:10">
       <c r="B63" s="13" t="s">
         <v>80</v>
       </c>
@@ -4375,7 +4392,7 @@
       </c>
       <c r="J63" s="17"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10">
       <c r="B64" s="13" t="s">
         <v>81</v>
       </c>
@@ -4400,7 +4417,7 @@
       </c>
       <c r="J64" s="17"/>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:10">
       <c r="B65" s="13" t="s">
         <v>82</v>
       </c>
@@ -4423,7 +4440,7 @@
       </c>
       <c r="J65" s="17"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:10">
       <c r="B66" s="13" t="s">
         <v>83</v>
       </c>
@@ -4446,7 +4463,7 @@
       </c>
       <c r="J66" s="17"/>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:10">
       <c r="B67" s="13" t="s">
         <v>84</v>
       </c>
@@ -4469,7 +4486,7 @@
       </c>
       <c r="J67" s="17"/>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:10">
       <c r="B68" s="13" t="s">
         <v>85</v>
       </c>
@@ -4492,7 +4509,7 @@
       </c>
       <c r="J68" s="17"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:10">
       <c r="B69" s="13" t="s">
         <v>86</v>
       </c>
@@ -4517,7 +4534,7 @@
       </c>
       <c r="J69" s="17"/>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:10">
       <c r="B70" s="13" t="s">
         <v>87</v>
       </c>
@@ -4540,7 +4557,7 @@
       </c>
       <c r="J70" s="17"/>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:10">
       <c r="B71" s="13" t="s">
         <v>88</v>
       </c>
@@ -4563,7 +4580,7 @@
       </c>
       <c r="J71" s="17"/>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:10">
       <c r="B72" s="13" t="s">
         <v>89</v>
       </c>
@@ -4588,7 +4605,7 @@
       </c>
       <c r="J72" s="17"/>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:10">
       <c r="B73" s="13" t="s">
         <v>90</v>
       </c>
@@ -4612,7 +4629,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:10">
       <c r="B74" s="13"/>
       <c r="C74" s="41"/>
       <c r="D74" s="15"/>
@@ -4621,13 +4638,13 @@
       <c r="G74" s="3"/>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:10">
       <c r="B75" s="49" t="s">
         <v>164</v>
       </c>
       <c r="C75" s="41"/>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:10">
       <c r="B76" s="13" t="s">
         <v>41</v>
       </c>
@@ -4654,7 +4671,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:10">
       <c r="B77" s="13" t="s">
         <v>42</v>
       </c>
@@ -4681,7 +4698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:10">
       <c r="B78" s="13" t="s">
         <v>43</v>
       </c>
@@ -4708,7 +4725,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:10">
       <c r="B79" s="13" t="s">
         <v>44</v>
       </c>
@@ -4735,7 +4752,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:10">
       <c r="B80" s="13" t="s">
         <v>45</v>
       </c>
@@ -4762,7 +4779,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:10">
       <c r="B81" s="13" t="s">
         <v>46</v>
       </c>
@@ -4789,7 +4806,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:10">
       <c r="B82" s="13" t="s">
         <v>47</v>
       </c>
@@ -4816,7 +4833,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:10">
       <c r="B83" s="13" t="s">
         <v>48</v>
       </c>
@@ -4843,17 +4860,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:10">
       <c r="B84" s="13"/>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:10">
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:10">
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>

</xml_diff>